<commit_message>
Updates to Final Presentation
</commit_message>
<xml_diff>
--- a/Code/_Dennis_Sandbox/_Output/DAT 205-Group01-Model Analysis Results 202104010a.xlsx
+++ b/Code/_Dennis_Sandbox/_Output/DAT 205-Group01-Model Analysis Results 202104010a.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Data-Den\GitHub\Capstone\Code\_Dennis_Sandbox\_Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F66AD2C-DC57-4B8E-BD22-70C8D5083E1F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC94BC71-D71C-427F-A6BB-B15FEAF85F99}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FI Results 20210330a" sheetId="7" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="75">
   <si>
     <t>TOV</t>
   </si>
@@ -247,6 +247,18 @@
   </si>
   <si>
     <t>GAME_ID</t>
+  </si>
+  <si>
+    <t>Loss</t>
+  </si>
+  <si>
+    <t>Win</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Bad</t>
   </si>
 </sst>
 </file>
@@ -462,16 +474,16 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,13 +493,13 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFE8282"/>
+      <color rgb="FFBC0000"/>
       <color rgb="FF990000"/>
-      <color rgb="FFBC0000"/>
-      <color rgb="FFFE8282"/>
+      <color rgb="FFCC0000"/>
       <color rgb="FFFFDDDD"/>
       <color rgb="FFFF0000"/>
       <color rgb="FFFF4747"/>
-      <color rgb="FFCC0000"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1661,78 +1673,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1600" b="1" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Accuracy / F1-Score / Sensitivity / Specificity </a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1600" b="1" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>by Models Comparison</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-CA" sz="1200">
-              <a:effectLst/>
-            </a:endParaRPr>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -1740,9 +1681,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.16361859767529058"/>
-          <c:y val="0.15331414046080608"/>
+          <c:y val="6.2779141479351819E-2"/>
           <c:w val="0.79423037120359952"/>
-          <c:h val="0.66292357407376601"/>
+          <c:h val="0.75345857305522035"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -3796,6 +3737,576 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Prediction!$O$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Random Forest</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FE8282"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Prediction!$N$9:$N$12</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Specificity</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sensitivity</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>F1 score</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Prediction!$O$9:$O$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.97099999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95099999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.96099999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.96099999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CF17-4D2A-B3F5-E73339E88FD3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="1438203007"/>
+        <c:axId val="1438208415"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1438203007"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1438208415"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1438208415"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1438203007"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Prediction!$O$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Random Forest</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FE8282"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Prediction!$N$9:$N$12</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Specificity</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sensitivity</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>F1 score</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Prediction!$O$9:$O$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.97099999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95099999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.96099999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.96099999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6E64-42F0-BBAF-5AE2230AC989}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="1438203007"/>
+        <c:axId val="1438208415"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1438203007"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1438208415"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1438208415"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1438203007"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3963,6 +4474,80 @@
   <a:schemeClr val="accent3"/>
   <a:schemeClr val="accent4"/>
   <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
   <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
@@ -6519,6 +7104,1016 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -6596,6 +8191,182 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>67622</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>19708</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFEDB448-491B-4988-9EE2-857BFE73554E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="14735175"/>
+          <a:ext cx="6782747" cy="4715533"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>39043</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>38761</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0DA1273-1CCA-4D1C-89C6-005603795072}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="19592925"/>
+          <a:ext cx="6754168" cy="4734586"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>138</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>105727</xdr:colOff>
+      <xdr:row>167</xdr:row>
+      <xdr:rowOff>29234</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A11CDE49-AAA9-41AB-918D-A45D999AC3B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="24774525"/>
+          <a:ext cx="6820852" cy="4725059"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>170</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>29516</xdr:colOff>
+      <xdr:row>199</xdr:row>
+      <xdr:rowOff>29234</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CF256C8-3F04-4FDA-A09D-463830266A88}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="29956125"/>
+          <a:ext cx="6744641" cy="4725059"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -6710,6 +8481,80 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>384663</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>296740</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>60080</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A236C547-16C6-4B77-A679-821F2BD5ACEA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>366346</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>117231</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>278423</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>120162</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E88C3CA1-BB6A-4C5E-AB7F-648270F041FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7997,8 +9842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{628E91ED-A764-4DE3-A122-889DBEC793BF}">
   <dimension ref="A3:Y151"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="A132" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B171" sqref="B171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -10176,18 +12021,18 @@
       <c r="F57" s="3">
         <v>0.67236300000000004</v>
       </c>
-      <c r="K57" s="29" t="s">
+      <c r="K57" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="L57" s="30"/>
-      <c r="M57" s="29" t="s">
+      <c r="L57" s="34"/>
+      <c r="M57" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="N57" s="30"/>
-      <c r="O57" s="29" t="s">
+      <c r="N57" s="34"/>
+      <c r="O57" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="P57" s="30"/>
+      <c r="P57" s="34"/>
     </row>
     <row r="58" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
       <c r="D58" s="3">
@@ -17750,10 +19595,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:R85"/>
+  <dimension ref="A2:U85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView topLeftCell="M1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="U56" sqref="U56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -17767,12 +19612,12 @@
     <col min="15" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B2" s="16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B4" s="17" t="s">
         <v>44</v>
       </c>
@@ -17786,7 +19631,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>1</v>
       </c>
@@ -17829,7 +19674,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>2</v>
       </c>
@@ -17867,7 +19712,7 @@
         <v>0.73853400000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B7" s="19" t="s">
         <v>47</v>
       </c>
@@ -17877,15 +19722,18 @@
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
         <v>50</v>
       </c>
       <c r="C8" s="18">
         <v>72</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="O8" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B9" s="16" t="s">
         <v>48</v>
       </c>
@@ -17893,14 +19741,17 @@
         <f>C7-C6</f>
         <v>12</v>
       </c>
+      <c r="M9" s="16">
+        <v>1</v>
+      </c>
       <c r="N9" s="28" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="O9" s="10">
-        <v>0.96099999999999997</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+        <v>0.97099999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B10" s="16" t="s">
         <v>49</v>
       </c>
@@ -17909,14 +19760,17 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="D10" s="20"/>
+      <c r="M10" s="16">
+        <v>2</v>
+      </c>
       <c r="N10" s="28" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O10" s="10">
-        <v>0.96099999999999997</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+        <v>0.95099999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D11" s="22"/>
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
@@ -17926,14 +19780,17 @@
       <c r="J11" s="22"/>
       <c r="K11" s="22"/>
       <c r="L11" s="22"/>
+      <c r="M11" s="16">
+        <v>3</v>
+      </c>
       <c r="N11" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O11" s="10">
-        <v>0.95099999999999996</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+        <v>0.96099999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
@@ -17943,14 +19800,17 @@
       <c r="J12" s="22"/>
       <c r="K12" s="22"/>
       <c r="L12" s="22"/>
+      <c r="M12" s="16">
+        <v>4</v>
+      </c>
       <c r="N12" s="28" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="O12" s="10">
-        <v>0.97099999999999997</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+        <v>0.96099999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
       <c r="F13" s="22"/>
@@ -17960,8 +19820,16 @@
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
       <c r="L13" s="22"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N13" s="22"/>
+      <c r="O13" s="22"/>
+      <c r="P13" s="22"/>
+      <c r="Q13" s="22"/>
+      <c r="R13" s="22"/>
+      <c r="S13" s="22"/>
+      <c r="T13" s="22"/>
+      <c r="U13" s="22"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
       <c r="F14" s="22"/>
@@ -17971,8 +19839,16 @@
       <c r="J14" s="22"/>
       <c r="K14" s="22"/>
       <c r="L14" s="22"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N14" s="22"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="22"/>
+      <c r="R14" s="22"/>
+      <c r="S14" s="22"/>
+      <c r="T14" s="22"/>
+      <c r="U14" s="22"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
       <c r="F15" s="22"/>
@@ -17982,8 +19858,16 @@
       <c r="J15" s="22"/>
       <c r="K15" s="22"/>
       <c r="L15" s="22"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N15" s="22"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="22"/>
+      <c r="Q15" s="22"/>
+      <c r="R15" s="22"/>
+      <c r="S15" s="22"/>
+      <c r="T15" s="22"/>
+      <c r="U15" s="22"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
       <c r="F16" s="22"/>
@@ -17993,8 +19877,16 @@
       <c r="J16" s="22"/>
       <c r="K16" s="22"/>
       <c r="L16" s="22"/>
-    </row>
-    <row r="17" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="N16" s="22"/>
+      <c r="O16" s="22"/>
+      <c r="P16" s="22"/>
+      <c r="Q16" s="22"/>
+      <c r="R16" s="22"/>
+      <c r="S16" s="22"/>
+      <c r="T16" s="22"/>
+      <c r="U16" s="22"/>
+    </row>
+    <row r="17" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
       <c r="F17" s="22"/>
@@ -18004,8 +19896,16 @@
       <c r="J17" s="22"/>
       <c r="K17" s="22"/>
       <c r="L17" s="22"/>
-    </row>
-    <row r="18" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="N17" s="22"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="22"/>
+      <c r="R17" s="22"/>
+      <c r="S17" s="22"/>
+      <c r="T17" s="22"/>
+      <c r="U17" s="22"/>
+    </row>
+    <row r="18" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
@@ -18015,8 +19915,16 @@
       <c r="J18" s="22"/>
       <c r="K18" s="22"/>
       <c r="L18" s="22"/>
-    </row>
-    <row r="19" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="N18" s="22"/>
+      <c r="O18" s="22"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="22"/>
+      <c r="R18" s="22"/>
+      <c r="S18" s="22"/>
+      <c r="T18" s="22"/>
+      <c r="U18" s="22"/>
+    </row>
+    <row r="19" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
@@ -18026,8 +19934,16 @@
       <c r="J19" s="22"/>
       <c r="K19" s="22"/>
       <c r="L19" s="22"/>
-    </row>
-    <row r="20" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="N19" s="22"/>
+      <c r="O19" s="22"/>
+      <c r="P19" s="22"/>
+      <c r="Q19" s="22"/>
+      <c r="R19" s="22"/>
+      <c r="S19" s="22"/>
+      <c r="T19" s="22"/>
+      <c r="U19" s="22"/>
+    </row>
+    <row r="20" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
@@ -18037,8 +19953,16 @@
       <c r="J20" s="22"/>
       <c r="K20" s="22"/>
       <c r="L20" s="22"/>
-    </row>
-    <row r="21" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="N20" s="22"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="22"/>
+      <c r="Q20" s="22"/>
+      <c r="R20" s="22"/>
+      <c r="S20" s="22"/>
+      <c r="T20" s="22"/>
+      <c r="U20" s="22"/>
+    </row>
+    <row r="21" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D21" s="22"/>
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
@@ -18048,8 +19972,16 @@
       <c r="J21" s="22"/>
       <c r="K21" s="22"/>
       <c r="L21" s="22"/>
-    </row>
-    <row r="22" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="N21" s="22"/>
+      <c r="O21" s="22"/>
+      <c r="P21" s="22"/>
+      <c r="Q21" s="22"/>
+      <c r="R21" s="22"/>
+      <c r="S21" s="22"/>
+      <c r="T21" s="22"/>
+      <c r="U21" s="22"/>
+    </row>
+    <row r="22" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
@@ -18059,8 +19991,16 @@
       <c r="J22" s="22"/>
       <c r="K22" s="22"/>
       <c r="L22" s="22"/>
-    </row>
-    <row r="23" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="N22" s="22"/>
+      <c r="O22" s="22"/>
+      <c r="P22" s="22"/>
+      <c r="Q22" s="22"/>
+      <c r="R22" s="22"/>
+      <c r="S22" s="22"/>
+      <c r="T22" s="22"/>
+      <c r="U22" s="22"/>
+    </row>
+    <row r="23" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
       <c r="F23" s="22"/>
@@ -18070,8 +20010,16 @@
       <c r="J23" s="22"/>
       <c r="K23" s="22"/>
       <c r="L23" s="22"/>
-    </row>
-    <row r="24" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="N23" s="22"/>
+      <c r="O23" s="22"/>
+      <c r="P23" s="22"/>
+      <c r="Q23" s="22"/>
+      <c r="R23" s="22"/>
+      <c r="S23" s="22"/>
+      <c r="T23" s="22"/>
+      <c r="U23" s="22"/>
+    </row>
+    <row r="24" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
       <c r="F24" s="22"/>
@@ -18081,8 +20029,16 @@
       <c r="J24" s="22"/>
       <c r="K24" s="22"/>
       <c r="L24" s="22"/>
-    </row>
-    <row r="25" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="N24" s="22"/>
+      <c r="O24" s="22"/>
+      <c r="P24" s="22"/>
+      <c r="Q24" s="22"/>
+      <c r="R24" s="22"/>
+      <c r="S24" s="22"/>
+      <c r="T24" s="22"/>
+      <c r="U24" s="22"/>
+    </row>
+    <row r="25" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
       <c r="F25" s="22"/>
@@ -18092,8 +20048,16 @@
       <c r="J25" s="22"/>
       <c r="K25" s="22"/>
       <c r="L25" s="22"/>
-    </row>
-    <row r="26" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="N25" s="22"/>
+      <c r="O25" s="22"/>
+      <c r="P25" s="22"/>
+      <c r="Q25" s="22"/>
+      <c r="R25" s="22"/>
+      <c r="S25" s="22"/>
+      <c r="T25" s="22"/>
+      <c r="U25" s="22"/>
+    </row>
+    <row r="26" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D26" s="22"/>
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
@@ -18103,8 +20067,16 @@
       <c r="J26" s="22"/>
       <c r="K26" s="22"/>
       <c r="L26" s="22"/>
-    </row>
-    <row r="27" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="N26" s="22"/>
+      <c r="O26" s="22"/>
+      <c r="P26" s="22"/>
+      <c r="Q26" s="22"/>
+      <c r="R26" s="22"/>
+      <c r="S26" s="22"/>
+      <c r="T26" s="22"/>
+      <c r="U26" s="22"/>
+    </row>
+    <row r="27" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
       <c r="F27" s="22"/>
@@ -18114,8 +20086,16 @@
       <c r="J27" s="22"/>
       <c r="K27" s="22"/>
       <c r="L27" s="22"/>
-    </row>
-    <row r="28" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="N27" s="22"/>
+      <c r="O27" s="22"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="22"/>
+      <c r="S27" s="22"/>
+      <c r="T27" s="22"/>
+      <c r="U27" s="22"/>
+    </row>
+    <row r="28" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
       <c r="F28" s="22"/>
@@ -18125,8 +20105,16 @@
       <c r="J28" s="22"/>
       <c r="K28" s="22"/>
       <c r="L28" s="22"/>
-    </row>
-    <row r="29" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="N28" s="22"/>
+      <c r="O28" s="22"/>
+      <c r="P28" s="22"/>
+      <c r="Q28" s="22"/>
+      <c r="R28" s="22"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="22"/>
+      <c r="U28" s="22"/>
+    </row>
+    <row r="29" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
@@ -18136,8 +20124,46 @@
       <c r="J29" s="22"/>
       <c r="K29" s="22"/>
       <c r="L29" s="22"/>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N29" s="22"/>
+      <c r="O29" s="22"/>
+      <c r="P29" s="22"/>
+      <c r="Q29" s="22"/>
+      <c r="R29" s="22"/>
+      <c r="S29" s="22"/>
+      <c r="T29" s="22"/>
+      <c r="U29" s="22"/>
+    </row>
+    <row r="30" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="N30" s="22"/>
+      <c r="O30" s="22"/>
+      <c r="P30" s="22"/>
+      <c r="Q30" s="22"/>
+      <c r="R30" s="22"/>
+      <c r="S30" s="22"/>
+      <c r="T30" s="22"/>
+      <c r="U30" s="22"/>
+    </row>
+    <row r="31" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="N31" s="22"/>
+      <c r="O31" s="22"/>
+      <c r="P31" s="22"/>
+      <c r="Q31" s="22"/>
+      <c r="R31" s="22"/>
+      <c r="S31" s="22"/>
+      <c r="T31" s="22"/>
+      <c r="U31" s="22"/>
+    </row>
+    <row r="32" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="N32" s="22"/>
+      <c r="O32" s="22"/>
+      <c r="P32" s="22"/>
+      <c r="Q32" s="22"/>
+      <c r="R32" s="22"/>
+      <c r="S32" s="22"/>
+      <c r="T32" s="22"/>
+      <c r="U32" s="22"/>
+    </row>
+    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B33" s="17" t="s">
         <v>44</v>
       </c>
@@ -18148,8 +20174,16 @@
       <c r="E33" s="17" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N33" s="22"/>
+      <c r="O33" s="22"/>
+      <c r="P33" s="22"/>
+      <c r="Q33" s="22"/>
+      <c r="R33" s="22"/>
+      <c r="S33" s="22"/>
+      <c r="T33" s="22"/>
+      <c r="U33" s="22"/>
+    </row>
+    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B34" s="18" t="s">
         <v>45</v>
       </c>
@@ -18163,8 +20197,16 @@
         <f>C39</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N34" s="22"/>
+      <c r="O34" s="22"/>
+      <c r="P34" s="22"/>
+      <c r="Q34" s="22"/>
+      <c r="R34" s="22"/>
+      <c r="S34" s="22"/>
+      <c r="T34" s="22"/>
+      <c r="U34" s="22"/>
+    </row>
+    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B35" s="25" t="s">
         <v>57</v>
       </c>
@@ -18175,8 +20217,16 @@
         <v>12</v>
       </c>
       <c r="E35" s="18"/>
-    </row>
-    <row r="36" spans="2:12" ht="51" x14ac:dyDescent="0.25">
+      <c r="N35" s="22"/>
+      <c r="O35" s="22"/>
+      <c r="P35" s="22"/>
+      <c r="Q35" s="22"/>
+      <c r="R35" s="22"/>
+      <c r="S35" s="22"/>
+      <c r="T35" s="22"/>
+      <c r="U35" s="22"/>
+    </row>
+    <row r="36" spans="2:21" ht="51" x14ac:dyDescent="0.25">
       <c r="B36" s="19" t="s">
         <v>47</v>
       </c>
@@ -18185,8 +20235,26 @@
       </c>
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N36" s="22"/>
+      <c r="O36" s="22"/>
+      <c r="P36" s="22"/>
+      <c r="Q36" s="22"/>
+      <c r="R36" s="22"/>
+      <c r="S36" s="22"/>
+      <c r="T36" s="22"/>
+      <c r="U36" s="22"/>
+    </row>
+    <row r="37" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="N37" s="22"/>
+      <c r="O37" s="22"/>
+      <c r="P37" s="22"/>
+      <c r="Q37" s="22"/>
+      <c r="R37" s="22"/>
+      <c r="S37" s="22"/>
+      <c r="T37" s="22"/>
+      <c r="U37" s="22"/>
+    </row>
+    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
       <c r="E38" s="22"/>
       <c r="F38" s="22"/>
       <c r="G38" s="22"/>
@@ -18195,8 +20263,16 @@
       <c r="J38" s="22"/>
       <c r="K38" s="22"/>
       <c r="L38" s="22"/>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N38" s="22"/>
+      <c r="O38" s="22"/>
+      <c r="P38" s="22"/>
+      <c r="Q38" s="22"/>
+      <c r="R38" s="22"/>
+      <c r="S38" s="22"/>
+      <c r="T38" s="22"/>
+      <c r="U38" s="22"/>
+    </row>
+    <row r="39" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D39" s="22"/>
       <c r="E39" s="22"/>
       <c r="F39" s="22"/>
@@ -18206,8 +20282,16 @@
       <c r="J39" s="22"/>
       <c r="K39" s="22"/>
       <c r="L39" s="22"/>
-    </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N39" s="22"/>
+      <c r="O39" s="22"/>
+      <c r="P39" s="22"/>
+      <c r="Q39" s="22"/>
+      <c r="R39" s="22"/>
+      <c r="S39" s="22"/>
+      <c r="T39" s="22"/>
+      <c r="U39" s="22"/>
+    </row>
+    <row r="40" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D40" s="22"/>
       <c r="E40" s="22"/>
       <c r="F40" s="22"/>
@@ -18217,8 +20301,16 @@
       <c r="J40" s="22"/>
       <c r="K40" s="22"/>
       <c r="L40" s="22"/>
-    </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N40" s="22"/>
+      <c r="O40" s="22"/>
+      <c r="P40" s="22"/>
+      <c r="Q40" s="22"/>
+      <c r="R40" s="22"/>
+      <c r="S40" s="22"/>
+      <c r="T40" s="22"/>
+      <c r="U40" s="22"/>
+    </row>
+    <row r="41" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D41" s="22"/>
       <c r="E41" s="22"/>
       <c r="F41" s="22"/>
@@ -18228,8 +20320,16 @@
       <c r="J41" s="22"/>
       <c r="K41" s="22"/>
       <c r="L41" s="22"/>
-    </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N41" s="22"/>
+      <c r="O41" s="22"/>
+      <c r="P41" s="22"/>
+      <c r="Q41" s="22"/>
+      <c r="R41" s="22"/>
+      <c r="S41" s="22"/>
+      <c r="T41" s="22"/>
+      <c r="U41" s="22"/>
+    </row>
+    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D42" s="22"/>
       <c r="E42" s="22"/>
       <c r="F42" s="22"/>
@@ -18239,8 +20339,16 @@
       <c r="J42" s="22"/>
       <c r="K42" s="22"/>
       <c r="L42" s="22"/>
-    </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N42" s="22"/>
+      <c r="O42" s="22"/>
+      <c r="P42" s="22"/>
+      <c r="Q42" s="22"/>
+      <c r="R42" s="22"/>
+      <c r="S42" s="22"/>
+      <c r="T42" s="22"/>
+      <c r="U42" s="22"/>
+    </row>
+    <row r="43" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D43" s="22"/>
       <c r="E43" s="22"/>
       <c r="F43" s="22"/>
@@ -18250,8 +20358,16 @@
       <c r="J43" s="22"/>
       <c r="K43" s="22"/>
       <c r="L43" s="22"/>
-    </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N43" s="22"/>
+      <c r="O43" s="22"/>
+      <c r="P43" s="22"/>
+      <c r="Q43" s="22"/>
+      <c r="R43" s="22"/>
+      <c r="S43" s="22"/>
+      <c r="T43" s="22"/>
+      <c r="U43" s="22"/>
+    </row>
+    <row r="44" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D44" s="22"/>
       <c r="E44" s="22"/>
       <c r="F44" s="22"/>
@@ -18261,8 +20377,16 @@
       <c r="J44" s="22"/>
       <c r="K44" s="22"/>
       <c r="L44" s="22"/>
-    </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N44" s="22"/>
+      <c r="O44" s="22"/>
+      <c r="P44" s="22"/>
+      <c r="Q44" s="22"/>
+      <c r="R44" s="22"/>
+      <c r="S44" s="22"/>
+      <c r="T44" s="22"/>
+      <c r="U44" s="22"/>
+    </row>
+    <row r="45" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D45" s="22"/>
       <c r="E45" s="22"/>
       <c r="F45" s="22"/>
@@ -18272,8 +20396,16 @@
       <c r="J45" s="22"/>
       <c r="K45" s="22"/>
       <c r="L45" s="22"/>
-    </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N45" s="22"/>
+      <c r="O45" s="22"/>
+      <c r="P45" s="22"/>
+      <c r="Q45" s="22"/>
+      <c r="R45" s="22"/>
+      <c r="S45" s="22"/>
+      <c r="T45" s="22"/>
+      <c r="U45" s="22"/>
+    </row>
+    <row r="46" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D46" s="22"/>
       <c r="E46" s="22"/>
       <c r="F46" s="22"/>
@@ -18283,8 +20415,16 @@
       <c r="J46" s="22"/>
       <c r="K46" s="22"/>
       <c r="L46" s="22"/>
-    </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N46" s="22"/>
+      <c r="O46" s="22"/>
+      <c r="P46" s="22"/>
+      <c r="Q46" s="22"/>
+      <c r="R46" s="22"/>
+      <c r="S46" s="22"/>
+      <c r="T46" s="22"/>
+      <c r="U46" s="22"/>
+    </row>
+    <row r="47" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D47" s="22"/>
       <c r="E47" s="22"/>
       <c r="F47" s="22"/>
@@ -18294,8 +20434,16 @@
       <c r="J47" s="22"/>
       <c r="K47" s="22"/>
       <c r="L47" s="22"/>
-    </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N47" s="22"/>
+      <c r="O47" s="22"/>
+      <c r="P47" s="22"/>
+      <c r="Q47" s="22"/>
+      <c r="R47" s="22"/>
+      <c r="S47" s="22"/>
+      <c r="T47" s="22"/>
+      <c r="U47" s="22"/>
+    </row>
+    <row r="48" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D48" s="22"/>
       <c r="E48" s="22"/>
       <c r="F48" s="22"/>
@@ -18306,7 +20454,7 @@
       <c r="K48" s="22"/>
       <c r="L48" s="22"/>
     </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D49" s="22"/>
       <c r="E49" s="22"/>
       <c r="F49" s="22"/>
@@ -18317,7 +20465,7 @@
       <c r="K49" s="22"/>
       <c r="L49" s="22"/>
     </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D50" s="22"/>
       <c r="E50" s="22"/>
       <c r="F50" s="22"/>
@@ -18327,8 +20475,23 @@
       <c r="J50" s="22"/>
       <c r="K50" s="22"/>
       <c r="L50" s="22"/>
-    </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P50" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q50" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="R50" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="S50" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="T50" s="16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D51" s="22"/>
       <c r="E51" s="22"/>
       <c r="F51" s="22"/>
@@ -18338,8 +20501,26 @@
       <c r="J51" s="22"/>
       <c r="K51" s="22"/>
       <c r="L51" s="22"/>
-    </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O51" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="P51" s="16">
+        <v>22.9</v>
+      </c>
+      <c r="Q51" s="16">
+        <v>44.4</v>
+      </c>
+      <c r="R51" s="16">
+        <v>9</v>
+      </c>
+      <c r="S51" s="16">
+        <v>5.3</v>
+      </c>
+      <c r="T51" s="16">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="52" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D52" s="22"/>
       <c r="E52" s="22"/>
       <c r="F52" s="22"/>
@@ -18349,8 +20530,26 @@
       <c r="J52" s="22"/>
       <c r="K52" s="22"/>
       <c r="L52" s="22"/>
-    </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O52" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="P52" s="16">
+        <v>23.4</v>
+      </c>
+      <c r="Q52" s="16">
+        <v>51</v>
+      </c>
+      <c r="R52" s="16">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="S52" s="16">
+        <v>9.5</v>
+      </c>
+      <c r="T52" s="16">
+        <v>15.1</v>
+      </c>
+    </row>
+    <row r="53" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D53" s="22"/>
       <c r="E53" s="22"/>
       <c r="F53" s="22"/>
@@ -18360,8 +20559,28 @@
       <c r="J53" s="22"/>
       <c r="K53" s="22"/>
       <c r="L53" s="22"/>
-    </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P53" s="16">
+        <f>P52-P51</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q53" s="16">
+        <f t="shared" ref="Q53:T53" si="0">Q52-Q51</f>
+        <v>6.6000000000000014</v>
+      </c>
+      <c r="R53" s="16">
+        <f t="shared" si="0"/>
+        <v>-0.30000000000000071</v>
+      </c>
+      <c r="S53" s="16">
+        <f t="shared" si="0"/>
+        <v>4.2</v>
+      </c>
+      <c r="T53" s="16">
+        <f>-(T52-T51)</f>
+        <v>-0.90000000000000036</v>
+      </c>
+    </row>
+    <row r="54" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D54" s="22"/>
       <c r="E54" s="22"/>
       <c r="F54" s="22"/>
@@ -18371,8 +20590,27 @@
       <c r="J54" s="22"/>
       <c r="K54" s="22"/>
       <c r="L54" s="22"/>
-    </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O54" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="P54" s="16">
+        <f>P53</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q54" s="16">
+        <f>Q53</f>
+        <v>6.6000000000000014</v>
+      </c>
+      <c r="S54" s="16">
+        <f>S53</f>
+        <v>4.2</v>
+      </c>
+      <c r="U54" s="16">
+        <f>SUM(P54:T54)</f>
+        <v>11.3</v>
+      </c>
+    </row>
+    <row r="55" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D55" s="22"/>
       <c r="E55" s="22"/>
       <c r="F55" s="22"/>
@@ -18382,8 +20620,23 @@
       <c r="J55" s="22"/>
       <c r="K55" s="22"/>
       <c r="L55" s="22"/>
-    </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O55" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="R55" s="16">
+        <f>R53</f>
+        <v>-0.30000000000000071</v>
+      </c>
+      <c r="T55" s="16">
+        <f>T53</f>
+        <v>-0.90000000000000036</v>
+      </c>
+      <c r="U55" s="16">
+        <f>-SUM(P55:T55)</f>
+        <v>1.2000000000000011</v>
+      </c>
+    </row>
+    <row r="56" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D56" s="22"/>
       <c r="E56" s="22"/>
       <c r="F56" s="22"/>
@@ -18393,8 +20646,12 @@
       <c r="J56" s="22"/>
       <c r="K56" s="22"/>
       <c r="L56" s="22"/>
-    </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="U56" s="16">
+        <f>U54/U55</f>
+        <v>9.416666666666659</v>
+      </c>
+    </row>
+    <row r="57" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D57" s="22"/>
       <c r="E57" s="22"/>
       <c r="F57" s="22"/>
@@ -18405,7 +20662,7 @@
       <c r="K57" s="22"/>
       <c r="L57" s="22"/>
     </row>
-    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B61" s="17" t="s">
         <v>44</v>
       </c>
@@ -18417,7 +20674,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B62" s="25" t="s">
         <v>57</v>
       </c>
@@ -18429,7 +20686,7 @@
       </c>
       <c r="E62" s="18"/>
     </row>
-    <row r="63" spans="2:12" ht="51" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:21" ht="51" x14ac:dyDescent="0.25">
       <c r="B63" s="19" t="s">
         <v>47</v>
       </c>
@@ -18661,8 +20918,8 @@
       <c r="L85" s="22"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N9:N12">
-    <sortCondition ref="N9:N12"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M9:O12">
+    <sortCondition ref="M9:M12"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -18681,190 +20938,190 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="15" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J15" s="34" t="s">
+      <c r="J15" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="K15" s="31" t="s">
+      <c r="K15" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="L15" s="31" t="s">
+      <c r="L15" s="29" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="16" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J16" s="33" t="s">
+      <c r="J16" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="K16" s="32" t="s">
+      <c r="K16" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="L16" s="32" t="s">
+      <c r="L16" s="30" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="31" t="s">
+      <c r="D22" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="31" t="s">
+      <c r="E22" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="F22" s="31" t="s">
+      <c r="F22" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="G22" s="31" t="s">
+      <c r="G22" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="H22" s="31" t="s">
+      <c r="H22" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="I22" s="31" t="s">
+      <c r="I22" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="J22" s="31" t="s">
+      <c r="J22" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="K22" s="31" t="s">
+      <c r="K22" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="L22" s="31" t="s">
+      <c r="L22" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="M22" s="31" t="s">
+      <c r="M22" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="N22" s="31" t="s">
+      <c r="N22" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="O22" s="31" t="s">
+      <c r="O22" s="29" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="32" t="s">
+      <c r="B23" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="32">
+      <c r="C23" s="30">
         <v>38.133333333333297</v>
       </c>
-      <c r="D23" s="32">
+      <c r="D23" s="30">
         <v>6</v>
       </c>
-      <c r="E23" s="32">
+      <c r="E23" s="30">
         <v>13</v>
       </c>
-      <c r="F23" s="32">
+      <c r="F23" s="30">
         <v>0.46200000000000002</v>
       </c>
-      <c r="G23" s="32">
+      <c r="G23" s="30">
         <v>2</v>
       </c>
-      <c r="H23" s="32">
+      <c r="H23" s="30">
         <v>6</v>
       </c>
-      <c r="I23" s="32">
+      <c r="I23" s="30">
         <v>0.33299999999999902</v>
       </c>
-      <c r="J23" s="32">
+      <c r="J23" s="30">
         <v>0</v>
       </c>
-      <c r="K23" s="32">
+      <c r="K23" s="30">
         <v>0</v>
       </c>
-      <c r="L23" s="32">
+      <c r="L23" s="30">
         <v>0</v>
       </c>
-      <c r="M23" s="32">
+      <c r="M23" s="30">
         <v>0</v>
       </c>
-      <c r="N23" s="32">
+      <c r="N23" s="30">
         <v>6</v>
       </c>
-      <c r="O23" s="32">
+      <c r="O23" s="30">
         <v>6</v>
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="31" t="s">
+      <c r="C25" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="D25" s="31" t="s">
+      <c r="D25" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="E25" s="31" t="s">
+      <c r="E25" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="F25" s="31" t="s">
+      <c r="F25" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="G25" s="31" t="s">
+      <c r="G25" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="H25" s="31" t="s">
+      <c r="H25" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="I25" s="31" t="s">
+      <c r="I25" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="J25" s="31" t="s">
+      <c r="J25" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="K25" s="31" t="s">
+      <c r="K25" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="L25" s="31" t="s">
+      <c r="L25" s="29" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="32">
+      <c r="B26" s="30">
         <v>10</v>
       </c>
-      <c r="C26" s="32">
+      <c r="C26" s="30">
         <v>5</v>
       </c>
-      <c r="D26" s="32">
+      <c r="D26" s="30">
         <v>6</v>
       </c>
-      <c r="E26" s="32">
+      <c r="E26" s="30">
         <v>0</v>
       </c>
-      <c r="F26" s="32">
+      <c r="F26" s="30">
         <v>1</v>
       </c>
-      <c r="G26" s="32">
+      <c r="G26" s="30">
         <v>5</v>
       </c>
-      <c r="H26" s="32">
+      <c r="H26" s="30">
         <v>1</v>
       </c>
-      <c r="I26" s="32">
+      <c r="I26" s="30">
         <v>14</v>
       </c>
-      <c r="J26" s="32">
+      <c r="J26" s="30">
         <v>41</v>
       </c>
-      <c r="K26" s="32">
+      <c r="K26" s="30">
         <v>1</v>
       </c>
-      <c r="L26" s="32">
+      <c r="L26" s="30">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="C28" s="31" t="s">
+      <c r="C28" s="29" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>